<commit_message>
Update the english name for the account items
</commit_message>
<xml_diff>
--- a/src/resource/balancesheet-sample.xlsx
+++ b/src/resource/balancesheet-sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="507">
   <si>
     <t>流动资产</t>
   </si>
@@ -640,9 +640,6 @@
   </si>
   <si>
     <t>投资活动产生的现金流量净额</t>
-  </si>
-  <si>
-    <t>三、筹资活动产生的现金流量：</t>
   </si>
   <si>
     <t>吸收投资收到的现金</t>
@@ -1173,12 +1170,399 @@
   <si>
     <t>Current asset losses in suspense</t>
   </si>
+  <si>
+    <t>Loans and payments on behalf</t>
+  </si>
+  <si>
+    <t>Fixed assets-net book value</t>
+  </si>
+  <si>
+    <t>public welfare biological assets</t>
+  </si>
+  <si>
+    <t>right to share in circulation</t>
+  </si>
+  <si>
+    <t>Borrowings from central bank</t>
+  </si>
+  <si>
+    <t>Deposits from customers and interbank</t>
+  </si>
+  <si>
+    <t>Deposit funds</t>
+  </si>
+  <si>
+    <t>Derivative financial liabilities</t>
+  </si>
+  <si>
+    <t>Funds from sales of financial assets with repurchasement agreement</t>
+  </si>
+  <si>
+    <t>Handling charges and commissions payable</t>
+  </si>
+  <si>
+    <t>Interests payable</t>
+  </si>
+  <si>
+    <t>Margin payable</t>
+  </si>
+  <si>
+    <t>internal accouts receivable</t>
+  </si>
+  <si>
+    <t>Withholding Expenses</t>
+  </si>
+  <si>
+    <t>Estimated liquid Liability</t>
+  </si>
+  <si>
+    <t>Cession insurance premiums payable</t>
+  </si>
+  <si>
+    <t>Provision for insurance contracts</t>
+  </si>
+  <si>
+    <t>Funds received as agent of stock exchange</t>
+  </si>
+  <si>
+    <t>Funds received as stock underwrite</t>
+  </si>
+  <si>
+    <t>International ticket settlement</t>
+  </si>
+  <si>
+    <t>Domestic ticket settlement</t>
+  </si>
+  <si>
+    <t>Short term bonds payable</t>
+  </si>
+  <si>
+    <t>Other non-current liabilities</t>
+  </si>
+  <si>
+    <t>treasury stock</t>
+  </si>
+  <si>
+    <t>special reserve</t>
+  </si>
+  <si>
+    <t>Provision for normal risks</t>
+  </si>
+  <si>
+    <t>Unidentified loss of investment</t>
+  </si>
+  <si>
+    <t>Quasi distribution of cash dividend</t>
+  </si>
+  <si>
+    <t>Exchange differences on translating foreign operations</t>
+  </si>
+  <si>
+    <t>Total owners' equity belongs to parent company</t>
+  </si>
+  <si>
+    <t>Minority interest</t>
+  </si>
+  <si>
+    <t>Overall sales</t>
+  </si>
+  <si>
+    <t>其中：主营业务收入 Including:sales of main operations</t>
+  </si>
+  <si>
+    <t>Interest income</t>
+  </si>
+  <si>
+    <t>Insurance premiums earned</t>
+  </si>
+  <si>
+    <t>Handling charges and commissions income</t>
+  </si>
+  <si>
+    <t>real estate sales</t>
+  </si>
+  <si>
+    <t>Overall costs</t>
+  </si>
+  <si>
+    <t>Handling charges and commissions expenses</t>
+  </si>
+  <si>
+    <t>real estate sales costs</t>
+  </si>
+  <si>
+    <t>Refund of insurance premiums</t>
+  </si>
+  <si>
+    <t>Net payments for insurance claims</t>
+  </si>
+  <si>
+    <t>Net provision for insurance contracts</t>
+  </si>
+  <si>
+    <t>Commissions on insurance policies</t>
+  </si>
+  <si>
+    <t>Cession charges</t>
+  </si>
+  <si>
+    <t>Selling and distribution expenses</t>
+  </si>
+  <si>
+    <t>Gain or loss from changes in fair values</t>
+  </si>
+  <si>
+    <t>Investment income</t>
+  </si>
+  <si>
+    <t>Investment income from joint ventures and affiliates</t>
+  </si>
+  <si>
+    <t>Gain or loss on foreign exchange transactions</t>
+  </si>
+  <si>
+    <t>future income</t>
+  </si>
+  <si>
+    <t>trust income</t>
+  </si>
+  <si>
+    <t>subsidize revenue</t>
+  </si>
+  <si>
+    <t>profit from other operations</t>
+  </si>
+  <si>
+    <t>Including:Losses from disposal of non-current assets</t>
+  </si>
+  <si>
+    <t>Unaffirmed investment loss</t>
+  </si>
+  <si>
+    <t>Net profit belonging to parent company</t>
+  </si>
+  <si>
+    <t>Basic EPS</t>
+  </si>
+  <si>
+    <t>Earning per share(EPS)</t>
+  </si>
+  <si>
+    <t>Diluted EPS</t>
+  </si>
+  <si>
+    <t>Other consolidated income</t>
+  </si>
+  <si>
+    <t>Total consolidated income</t>
+  </si>
+  <si>
+    <t>Consolidated income belonging to parent company</t>
+  </si>
+  <si>
+    <t>Consolidated income belonging to Minority shareholders</t>
+  </si>
+  <si>
+    <t>Customer deposits and interbank deposits net increase</t>
+  </si>
+  <si>
+    <t>To other financial institutions borrowing funds net increase</t>
+  </si>
+  <si>
+    <t>Cash received from investment</t>
+  </si>
+  <si>
+    <t>Cash received from loan</t>
+  </si>
+  <si>
+    <t>Cash received from issuing bonds</t>
+  </si>
+  <si>
+    <t>Cash received relating to other financing activities</t>
+  </si>
+  <si>
+    <t>Cash inflow from financing activities</t>
+  </si>
+  <si>
+    <t>Cash paid for debts</t>
+  </si>
+  <si>
+    <t>The distribution of dividends, profits or interest paid in cash</t>
+  </si>
+  <si>
+    <t>Sub total of cash outflows from financing activities</t>
+  </si>
+  <si>
+    <t>Net increase in pledge loans</t>
+  </si>
+  <si>
+    <t>Increase the pledge and deposit paid in cash</t>
+  </si>
+  <si>
+    <t>Have net cash payment of subsidiaries and other business units</t>
+  </si>
+  <si>
+    <t>Cash received from minority shareholder investment by subsidiary</t>
+  </si>
+  <si>
+    <t>Net increase in placements from banks and other financial institutions</t>
+  </si>
+  <si>
+    <t>Premiums received from original insurance contracts</t>
+  </si>
+  <si>
+    <t>Net cash received from reinsurance business</t>
+  </si>
+  <si>
+    <t>Interest, handling charges and commission received</t>
+  </si>
+  <si>
+    <t>Tax rebates received</t>
+  </si>
+  <si>
+    <t>Net increase in deposits from policyholders</t>
+  </si>
+  <si>
+    <t>Net increase from disposal of tradable financial assets</t>
+  </si>
+  <si>
+    <t>Net increase in repurchase business capital</t>
+  </si>
+  <si>
+    <t>Net increase in loans and advances to customers</t>
+  </si>
+  <si>
+    <t>Net increase in deposits with central bank and other financial institutions</t>
+  </si>
+  <si>
+    <t>Original insurance contract claims paid</t>
+  </si>
+  <si>
+    <t>Interest, handling charges and commissions paid</t>
+  </si>
+  <si>
+    <t>Policyholder Dividend Paid</t>
+  </si>
+  <si>
+    <t>Cash paid for other financing activities</t>
+  </si>
+  <si>
+    <t>Assets depreciation reserves</t>
+  </si>
+  <si>
+    <t>Net cash received from disposal of subsidiaries and other business units</t>
+  </si>
+  <si>
+    <t>Minority Stockholder's Interest</t>
+  </si>
+  <si>
+    <t>Unconfirmed investment losses</t>
+  </si>
+  <si>
+    <t>Fixed assets depreciation, depletion of oil and gas assets depreciation, production materials</t>
+  </si>
+  <si>
+    <t>amortization of intangible assets</t>
+  </si>
+  <si>
+    <t>Increase in accrued expenses</t>
+  </si>
+  <si>
+    <t>Disposal of fixed assets, intangible assets and other long-term assets loss</t>
+  </si>
+  <si>
+    <t>Loss of scrapped fixed assets</t>
+  </si>
+  <si>
+    <t>Changes in the fair value of the loss</t>
+  </si>
+  <si>
+    <t>Increase in deferred income</t>
+  </si>
+  <si>
+    <t>Estimated liabilities</t>
+  </si>
+  <si>
+    <t>financial expenses</t>
+  </si>
+  <si>
+    <t>investment losses</t>
+  </si>
+  <si>
+    <t>Reduction of deferred income tax assets</t>
+  </si>
+  <si>
+    <t>Deferred income tax liabilities increased</t>
+  </si>
+  <si>
+    <t>The decrease of inventory</t>
+  </si>
+  <si>
+    <t>Decrease in operating receivables</t>
+  </si>
+  <si>
+    <t>Increase in operating payables</t>
+  </si>
+  <si>
+    <t>Has been completed and not yet settled in paragraph reduction</t>
+  </si>
+  <si>
+    <t>Have not yet completed payment settlement increase</t>
+  </si>
+  <si>
+    <t>Generated from operating activities net cash flow</t>
+  </si>
+  <si>
+    <t>The debt is converted into capital</t>
+  </si>
+  <si>
+    <t>The Switching Company bonds due within one year</t>
+  </si>
+  <si>
+    <t>fixed assets under financing lease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash at end of period/closing cash balance </t>
+  </si>
+  <si>
+    <t>cash at the beginning of the period</t>
+  </si>
+  <si>
+    <t>cash equivalents at the end of the period</t>
+  </si>
+  <si>
+    <t>cash equivalents at the beginning of the period</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Amortization of long-term prepayment(prepaid expenses)</t>
+  </si>
+  <si>
+    <t>Decrease in prepaid expense(prepaid and deferred expenses)</t>
+  </si>
+  <si>
+    <t>Net cash flow financing activities</t>
+  </si>
+  <si>
+    <t>三、筹资活动产生的现金流量：Cash flows from financing activities</t>
+  </si>
+  <si>
+    <t>Received reduce and deposit cash pledge</t>
+  </si>
+  <si>
+    <t>Other non current assets</t>
+  </si>
+  <si>
+    <t>Other long-term investment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1218,6 +1602,24 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -1264,7 +1666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1288,20 +1690,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -1322,6 +1712,26 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1626,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,35 +2054,35 @@
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C1" s="11">
+        <v>256</v>
+      </c>
+      <c r="C1" s="9">
         <v>39082</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E1" s="9">
         <v>41912</v>
       </c>
-      <c r="F1" s="11">
+      <c r="F1" s="9">
         <v>41820</v>
       </c>
-      <c r="G1" s="11">
+      <c r="G1" s="9">
         <v>41729</v>
       </c>
-      <c r="H1" s="11">
+      <c r="H1" s="9">
         <v>41639</v>
       </c>
-      <c r="I1" s="11">
+      <c r="I1" s="9">
         <v>41547</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
         <v>115</v>
@@ -1684,18 +2094,18 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9" t="s">
+      <c r="A3" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1703,7 +2113,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C4">
         <v>3668680</v>
@@ -1732,7 +2142,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C5">
         <v>1049070</v>
@@ -1761,7 +2171,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1790,7 +2200,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C7">
         <v>193711</v>
@@ -1819,7 +2229,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1848,7 +2258,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1877,7 +2287,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -1906,7 +2316,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -1935,7 +2345,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1964,7 +2374,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1993,7 +2403,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2022,7 +2432,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C15">
         <v>229.29</v>
@@ -2051,7 +2461,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -2080,7 +2490,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2109,7 +2519,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -2138,7 +2548,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2167,7 +2577,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C20">
         <v>116362</v>
@@ -2196,7 +2606,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -2225,7 +2635,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C22">
         <v>418913</v>
@@ -2254,7 +2664,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -2283,7 +2693,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2312,7 +2722,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -2341,7 +2751,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -2370,7 +2780,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -2399,7 +2809,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -2424,24 +2834,27 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="9" t="s">
+      <c r="A29" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
+      <c r="B30" t="s">
+        <v>378</v>
+      </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
@@ -2469,7 +2882,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C31">
         <v>272114</v>
@@ -2498,7 +2911,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -2527,7 +2940,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -2556,7 +2969,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C34">
         <v>118587</v>
@@ -2584,6 +2997,9 @@
       <c r="A35" t="s">
         <v>33</v>
       </c>
+      <c r="B35" t="s">
+        <v>506</v>
+      </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
@@ -2611,7 +3027,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C36">
         <v>7708.96</v>
@@ -2640,7 +3056,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C37">
         <v>77272.3</v>
@@ -2669,7 +3085,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C38">
         <v>29116.9</v>
@@ -2698,7 +3114,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C39">
         <v>48155.4</v>
@@ -2727,7 +3143,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -2755,6 +3171,9 @@
       <c r="A41" t="s">
         <v>39</v>
       </c>
+      <c r="B41" t="s">
+        <v>379</v>
+      </c>
       <c r="C41">
         <v>48155.4</v>
       </c>
@@ -2782,7 +3201,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C42">
         <v>24654.6</v>
@@ -2811,7 +3230,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
@@ -2840,7 +3259,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -2869,7 +3288,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -2897,6 +3316,9 @@
       <c r="A46" t="s">
         <v>44</v>
       </c>
+      <c r="B46" t="s">
+        <v>380</v>
+      </c>
       <c r="C46" t="s">
         <v>4</v>
       </c>
@@ -2924,7 +3346,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -2953,7 +3375,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C48">
         <v>12556.8</v>
@@ -2982,7 +3404,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
@@ -3011,7 +3433,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C50">
         <v>22535.7</v>
@@ -3037,10 +3459,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
@@ -3068,6 +3490,9 @@
       <c r="A52" t="s">
         <v>50</v>
       </c>
+      <c r="B52" t="s">
+        <v>381</v>
+      </c>
       <c r="C52" t="s">
         <v>4</v>
       </c>
@@ -3095,7 +3520,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C53">
         <v>6911.02</v>
@@ -3123,6 +3548,9 @@
       <c r="A54" t="s">
         <v>52</v>
       </c>
+      <c r="B54" t="s">
+        <v>505</v>
+      </c>
       <c r="C54">
         <v>431905</v>
       </c>
@@ -3150,7 +3578,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -3179,7 +3607,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C56">
         <v>6392090</v>
@@ -3204,18 +3632,18 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="9" t="s">
+      <c r="A57" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3223,7 +3651,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C58">
         <v>5023.3500000000004</v>
@@ -3251,6 +3679,9 @@
       <c r="A59" t="s">
         <v>58</v>
       </c>
+      <c r="B59" t="s">
+        <v>382</v>
+      </c>
       <c r="C59" t="s">
         <v>4</v>
       </c>
@@ -3277,6 +3708,9 @@
       <c r="A60" t="s">
         <v>59</v>
       </c>
+      <c r="B60" t="s">
+        <v>383</v>
+      </c>
       <c r="C60" t="s">
         <v>4</v>
       </c>
@@ -3303,6 +3737,9 @@
       <c r="A61" t="s">
         <v>60</v>
       </c>
+      <c r="B61" t="s">
+        <v>384</v>
+      </c>
       <c r="C61" t="s">
         <v>4</v>
       </c>
@@ -3330,7 +3767,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C62">
         <v>24902.2</v>
@@ -3358,6 +3795,9 @@
       <c r="A63" t="s">
         <v>62</v>
       </c>
+      <c r="B63" t="s">
+        <v>385</v>
+      </c>
       <c r="C63" t="s">
         <v>4</v>
       </c>
@@ -3385,7 +3825,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
@@ -3414,7 +3854,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C65" t="s">
         <v>4</v>
@@ -3443,7 +3883,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C66" t="s">
         <v>4</v>
@@ -3471,6 +3911,9 @@
       <c r="A67" t="s">
         <v>66</v>
       </c>
+      <c r="B67" t="s">
+        <v>386</v>
+      </c>
       <c r="C67">
         <v>230044</v>
       </c>
@@ -3497,6 +3940,9 @@
       <c r="A68" t="s">
         <v>67</v>
       </c>
+      <c r="B68" t="s">
+        <v>387</v>
+      </c>
       <c r="C68" t="s">
         <v>4</v>
       </c>
@@ -3521,10 +3967,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B69" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C69">
         <v>65238.2</v>
@@ -3550,10 +3996,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B70" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C70">
         <v>69770.600000000006</v>
@@ -3581,6 +4027,9 @@
       <c r="A71" t="s">
         <v>70</v>
       </c>
+      <c r="B71" t="s">
+        <v>388</v>
+      </c>
       <c r="C71">
         <v>5224.08</v>
       </c>
@@ -3608,7 +4057,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C72" t="s">
         <v>4</v>
@@ -3637,7 +4086,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C73" t="s">
         <v>4</v>
@@ -3665,6 +4114,9 @@
       <c r="A74" t="s">
         <v>73</v>
       </c>
+      <c r="B74" t="s">
+        <v>389</v>
+      </c>
       <c r="C74" t="s">
         <v>4</v>
       </c>
@@ -3691,6 +4143,9 @@
       <c r="A75" t="s">
         <v>74</v>
       </c>
+      <c r="B75" t="s">
+        <v>390</v>
+      </c>
       <c r="C75" t="s">
         <v>4</v>
       </c>
@@ -3717,6 +4172,9 @@
       <c r="A76" t="s">
         <v>75</v>
       </c>
+      <c r="B76" t="s">
+        <v>306</v>
+      </c>
       <c r="C76" t="s">
         <v>4</v>
       </c>
@@ -3743,6 +4201,9 @@
       <c r="A77" t="s">
         <v>76</v>
       </c>
+      <c r="B77" t="s">
+        <v>391</v>
+      </c>
       <c r="C77" t="s">
         <v>4</v>
       </c>
@@ -3769,6 +4230,9 @@
       <c r="A78" t="s">
         <v>77</v>
       </c>
+      <c r="B78" t="s">
+        <v>392</v>
+      </c>
       <c r="C78" t="s">
         <v>4</v>
       </c>
@@ -3795,6 +4259,9 @@
       <c r="A79" t="s">
         <v>78</v>
       </c>
+      <c r="B79" t="s">
+        <v>393</v>
+      </c>
       <c r="C79" t="s">
         <v>4</v>
       </c>
@@ -3821,6 +4288,9 @@
       <c r="A80" t="s">
         <v>79</v>
       </c>
+      <c r="B80" s="21" t="s">
+        <v>394</v>
+      </c>
       <c r="C80" t="s">
         <v>4</v>
       </c>
@@ -3847,6 +4317,9 @@
       <c r="A81" t="s">
         <v>80</v>
       </c>
+      <c r="B81" t="s">
+        <v>395</v>
+      </c>
       <c r="C81">
         <v>4182670</v>
       </c>
@@ -3873,6 +4346,9 @@
       <c r="A82" t="s">
         <v>81</v>
       </c>
+      <c r="B82" t="s">
+        <v>396</v>
+      </c>
       <c r="C82">
         <v>3057.07</v>
       </c>
@@ -3899,6 +4375,9 @@
       <c r="A83" t="s">
         <v>82</v>
       </c>
+      <c r="B83" t="s">
+        <v>397</v>
+      </c>
       <c r="C83" t="s">
         <v>4</v>
       </c>
@@ -3925,6 +4404,9 @@
       <c r="A84" t="s">
         <v>83</v>
       </c>
+      <c r="B84" t="s">
+        <v>398</v>
+      </c>
       <c r="C84" t="s">
         <v>4</v>
       </c>
@@ -3952,7 +4434,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C85" t="s">
         <v>4</v>
@@ -3980,6 +4462,9 @@
       <c r="A86" t="s">
         <v>85</v>
       </c>
+      <c r="B86" t="s">
+        <v>399</v>
+      </c>
       <c r="C86" t="s">
         <v>4</v>
       </c>
@@ -4007,7 +4492,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C87" t="s">
         <v>4</v>
@@ -4036,7 +4521,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
@@ -4065,7 +4550,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C89" t="s">
         <v>4</v>
@@ -4090,18 +4575,18 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="12" t="s">
-        <v>311</v>
-      </c>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="12" t="s">
+      <c r="A90" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
       <c r="I90" s="1"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -4109,7 +4594,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C91" s="6">
         <v>20093.400000000001</v>
@@ -4138,7 +4623,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C92" s="4">
         <v>195000</v>
@@ -4167,7 +4652,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>4</v>
@@ -4196,7 +4681,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>4</v>
@@ -4225,7 +4710,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C95" s="6">
         <v>2903</v>
@@ -4254,7 +4739,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C96" s="4">
         <v>5683.82</v>
@@ -4282,6 +4767,9 @@
       <c r="A97" t="s">
         <v>96</v>
       </c>
+      <c r="B97" t="s">
+        <v>400</v>
+      </c>
       <c r="C97" s="6">
         <v>195883</v>
       </c>
@@ -4309,7 +4797,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>4</v>
@@ -4338,7 +4826,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C99" s="6">
         <v>5005500</v>
@@ -4363,18 +4851,18 @@
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="12" t="s">
+      <c r="A100" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="B100" s="18"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="18"/>
       <c r="I100" s="1"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4382,7 +4870,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C101" s="6">
         <v>298150</v>
@@ -4411,7 +4899,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C102" s="4">
         <v>619567</v>
@@ -4439,6 +4927,9 @@
       <c r="A103" t="s">
         <v>102</v>
       </c>
+      <c r="B103" t="s">
+        <v>401</v>
+      </c>
       <c r="C103" s="8" t="s">
         <v>4</v>
       </c>
@@ -4465,6 +4956,9 @@
       <c r="A104" t="s">
         <v>103</v>
       </c>
+      <c r="B104" t="s">
+        <v>402</v>
+      </c>
       <c r="C104" s="7" t="s">
         <v>4</v>
       </c>
@@ -4492,7 +4986,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C105" s="6">
         <v>73228.899999999994</v>
@@ -4520,6 +5014,9 @@
       <c r="A106" t="s">
         <v>105</v>
       </c>
+      <c r="B106" t="s">
+        <v>403</v>
+      </c>
       <c r="C106" s="4">
         <v>52697.3</v>
       </c>
@@ -4546,6 +5043,9 @@
       <c r="A107" t="s">
         <v>106</v>
       </c>
+      <c r="B107" t="s">
+        <v>404</v>
+      </c>
       <c r="C107" s="8" t="s">
         <v>4</v>
       </c>
@@ -4573,7 +5073,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C108" s="4">
         <v>205549</v>
@@ -4601,6 +5101,9 @@
       <c r="A109" t="s">
         <v>108</v>
       </c>
+      <c r="B109" t="s">
+        <v>405</v>
+      </c>
       <c r="C109" s="8" t="s">
         <v>4</v>
       </c>
@@ -4627,6 +5130,9 @@
       <c r="A110" t="s">
         <v>109</v>
       </c>
+      <c r="B110" s="21" t="s">
+        <v>406</v>
+      </c>
       <c r="C110" s="7" t="s">
         <v>4</v>
       </c>
@@ -4653,6 +5159,9 @@
       <c r="A111" t="s">
         <v>110</v>
       </c>
+      <c r="B111" s="21" t="s">
+        <v>407</v>
+      </c>
       <c r="C111" s="6">
         <v>1249190</v>
       </c>
@@ -4679,6 +5188,9 @@
       <c r="A112" t="s">
         <v>111</v>
       </c>
+      <c r="B112" t="s">
+        <v>408</v>
+      </c>
       <c r="C112" s="4">
         <v>137397</v>
       </c>
@@ -4706,7 +5218,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C113" s="6">
         <v>1386590</v>
@@ -4735,7 +5247,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C114" s="4">
         <v>6392090</v>
@@ -4994,10 +5506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5007,150 +5519,178 @@
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C1" s="11">
+        <v>256</v>
+      </c>
+      <c r="C1" s="9">
         <v>41912</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>166</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="11" t="s">
+        <v>409</v>
+      </c>
       <c r="C3" s="6">
         <v>39451.800000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C4" s="4">
         <v>39451.800000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="22" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>411</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
+        <v>413</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>414</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>329</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="14" t="s">
+        <v>415</v>
+      </c>
       <c r="C10" s="4">
         <v>37868.800000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>124</v>
       </c>
       <c r="B11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C11" s="6">
         <v>30212.3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>336</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>416</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>417</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>335</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5158,7 +5698,10 @@
       <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="B17" t="s">
+        <v>419</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5166,7 +5709,10 @@
       <c r="A18" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="B18" t="s">
+        <v>420</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5174,7 +5720,10 @@
       <c r="A19" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5182,7 +5731,10 @@
       <c r="A20" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5191,9 +5743,9 @@
         <v>134</v>
       </c>
       <c r="B21" t="s">
-        <v>332</v>
-      </c>
-      <c r="C21" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5202,7 +5754,7 @@
         <v>135</v>
       </c>
       <c r="B22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C22" s="7">
         <v>103.84</v>
@@ -5212,6 +5764,9 @@
       <c r="A23" t="s">
         <v>136</v>
       </c>
+      <c r="B23" s="21" t="s">
+        <v>423</v>
+      </c>
       <c r="C23" s="6">
         <v>2210.62</v>
       </c>
@@ -5221,7 +5776,7 @@
         <v>137</v>
       </c>
       <c r="B24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C24" s="4">
         <v>3578.81</v>
@@ -5232,7 +5787,7 @@
         <v>138</v>
       </c>
       <c r="B25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C25" s="6">
         <v>2063.71</v>
@@ -5243,7 +5798,7 @@
         <v>139</v>
       </c>
       <c r="B26" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C26" s="7">
         <v>-300.45</v>
@@ -5253,7 +5808,10 @@
       <c r="A27" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="B27" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5261,6 +5819,9 @@
       <c r="A28" t="s">
         <v>141</v>
       </c>
+      <c r="B28" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="C28" s="7">
         <v>618.82000000000005</v>
       </c>
@@ -5269,7 +5830,10 @@
       <c r="A29" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="B29" s="21" t="s">
+        <v>426</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5277,7 +5841,10 @@
       <c r="A30" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="B30" s="21" t="s">
+        <v>427</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5285,7 +5852,10 @@
       <c r="A31" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="B31" s="21" t="s">
+        <v>428</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5293,7 +5863,10 @@
       <c r="A32" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="B32" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5301,7 +5874,10 @@
       <c r="A33" t="s">
         <v>146</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="B33" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5309,16 +5885,19 @@
       <c r="A34" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>339</v>
+      <c r="B35" s="11" t="s">
+        <v>338</v>
       </c>
       <c r="C35" s="6">
         <v>2201.8000000000002</v>
@@ -5329,7 +5908,7 @@
         <v>149</v>
       </c>
       <c r="B36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C36" s="7">
         <v>211.69</v>
@@ -5340,7 +5919,7 @@
         <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C37" s="8">
         <v>23.88</v>
@@ -5350,7 +5929,10 @@
       <c r="A38" t="s">
         <v>151</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5359,7 +5941,7 @@
         <v>152</v>
       </c>
       <c r="B39" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C39" s="6">
         <v>2389.6</v>
@@ -5370,7 +5952,7 @@
         <v>153</v>
       </c>
       <c r="B40" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C40" s="7">
         <v>168.29</v>
@@ -5380,16 +5962,19 @@
       <c r="A41" t="s">
         <v>154</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="B41" t="s">
+        <v>433</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B42" s="18" t="s">
-        <v>343</v>
+      <c r="B42" s="14" t="s">
+        <v>342</v>
       </c>
       <c r="C42" s="4">
         <v>2221.31</v>
@@ -5399,6 +5984,9 @@
       <c r="A43" t="s">
         <v>156</v>
       </c>
+      <c r="B43" t="s">
+        <v>434</v>
+      </c>
       <c r="C43" s="6">
         <v>2141.65</v>
       </c>
@@ -5408,23 +5996,28 @@
         <v>157</v>
       </c>
       <c r="B44" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C44" s="7">
         <v>79.66</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B45" s="20"/>
+      <c r="B45" s="16" t="s">
+        <v>436</v>
+      </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>159</v>
       </c>
+      <c r="B46" t="s">
+        <v>435</v>
+      </c>
       <c r="C46" s="7" t="s">
         <v>160</v>
       </c>
@@ -5433,24 +6026,31 @@
       <c r="A47" t="s">
         <v>161</v>
       </c>
+      <c r="B47" t="s">
+        <v>437</v>
+      </c>
       <c r="C47" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="B48" s="18"/>
+      <c r="B48" s="14" t="s">
+        <v>438</v>
+      </c>
       <c r="C48" s="7">
         <v>-439.5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B49" s="15"/>
+      <c r="B49" s="11" t="s">
+        <v>439</v>
+      </c>
       <c r="C49" s="6">
         <v>1781.81</v>
       </c>
@@ -5459,6 +6059,9 @@
       <c r="A50" t="s">
         <v>164</v>
       </c>
+      <c r="B50" t="s">
+        <v>440</v>
+      </c>
       <c r="C50" s="4">
         <v>1702.15</v>
       </c>
@@ -5466,6 +6069,9 @@
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>165</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>441</v>
       </c>
       <c r="C51" s="8">
         <v>79.66</v>
@@ -5522,6 +6128,7 @@
     <hyperlink ref="A49" r:id="rId47" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;type=cinst81"/>
     <hyperlink ref="A50" r:id="rId48" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;type=cinst82"/>
     <hyperlink ref="A51" r:id="rId49" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;type=cinst83"/>
+    <hyperlink ref="E4" r:id="rId50" display="http://www.baidu.com/s?wd=%E4%B8%BB%E8%90%A5%E4%B8%9A%E5%8A%A1%E6%94%B6%E5%85%A5&amp;hl_tag=textlink&amp;tn=SE_hldp01350_v6v6zkg6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5531,8 +6138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5549,27 +6156,27 @@
         <v>167</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C1" s="11">
+        <v>256</v>
+      </c>
+      <c r="C1" s="9">
         <v>41912</v>
       </c>
-      <c r="D1" s="11">
+      <c r="D1" s="9">
         <v>41820</v>
       </c>
-      <c r="E1" s="11">
+      <c r="E1" s="9">
         <v>41729</v>
       </c>
-      <c r="F1" s="11">
+      <c r="F1" s="9">
         <v>41639</v>
       </c>
-      <c r="G1" s="11">
+      <c r="G1" s="9">
         <v>41547</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -5579,14 +6186,14 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="A3" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -5594,7 +6201,7 @@
         <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C4" s="4">
         <v>48245.5</v>
@@ -5616,6 +6223,9 @@
       <c r="A5" t="s">
         <v>169</v>
       </c>
+      <c r="B5" t="s">
+        <v>442</v>
+      </c>
       <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
@@ -5636,6 +6246,9 @@
       <c r="A6" t="s">
         <v>170</v>
       </c>
+      <c r="B6" t="s">
+        <v>382</v>
+      </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
@@ -5656,6 +6269,9 @@
       <c r="A7" t="s">
         <v>171</v>
       </c>
+      <c r="B7" t="s">
+        <v>443</v>
+      </c>
       <c r="C7" s="8" t="s">
         <v>4</v>
       </c>
@@ -5676,6 +6292,9 @@
       <c r="A8" t="s">
         <v>172</v>
       </c>
+      <c r="B8" t="s">
+        <v>457</v>
+      </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
@@ -5696,6 +6315,9 @@
       <c r="A9" t="s">
         <v>173</v>
       </c>
+      <c r="B9" t="s">
+        <v>458</v>
+      </c>
       <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
@@ -5716,6 +6338,9 @@
       <c r="A10" t="s">
         <v>174</v>
       </c>
+      <c r="B10" t="s">
+        <v>461</v>
+      </c>
       <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
@@ -5736,6 +6361,9 @@
       <c r="A11" t="s">
         <v>175</v>
       </c>
+      <c r="B11" t="s">
+        <v>462</v>
+      </c>
       <c r="C11" s="8" t="s">
         <v>4</v>
       </c>
@@ -5756,6 +6384,9 @@
       <c r="A12" t="s">
         <v>176</v>
       </c>
+      <c r="B12" t="s">
+        <v>459</v>
+      </c>
       <c r="C12" s="7" t="s">
         <v>4</v>
       </c>
@@ -5776,6 +6407,9 @@
       <c r="A13" t="s">
         <v>177</v>
       </c>
+      <c r="B13" s="23" t="s">
+        <v>456</v>
+      </c>
       <c r="C13" s="8" t="s">
         <v>4</v>
       </c>
@@ -5796,6 +6430,9 @@
       <c r="A14" t="s">
         <v>178</v>
       </c>
+      <c r="B14" t="s">
+        <v>463</v>
+      </c>
       <c r="C14" s="7" t="s">
         <v>4</v>
       </c>
@@ -5812,9 +6449,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>179</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>460</v>
       </c>
       <c r="C15" s="8">
         <v>48.65</v>
@@ -5837,7 +6477,7 @@
         <v>180</v>
       </c>
       <c r="B16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C16" s="7">
         <v>115.85</v>
@@ -5860,7 +6500,7 @@
         <v>181</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C17" s="6">
         <v>48410</v>
@@ -5883,7 +6523,7 @@
         <v>182</v>
       </c>
       <c r="B18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C18" s="4">
         <v>31048.3</v>
@@ -5905,6 +6545,9 @@
       <c r="A19" t="s">
         <v>183</v>
       </c>
+      <c r="B19" t="s">
+        <v>464</v>
+      </c>
       <c r="C19" s="8" t="s">
         <v>4</v>
       </c>
@@ -5925,6 +6568,9 @@
       <c r="A20" t="s">
         <v>184</v>
       </c>
+      <c r="B20" t="s">
+        <v>465</v>
+      </c>
       <c r="C20" s="7" t="s">
         <v>4</v>
       </c>
@@ -5945,6 +6591,9 @@
       <c r="A21" t="s">
         <v>185</v>
       </c>
+      <c r="B21" t="s">
+        <v>466</v>
+      </c>
       <c r="C21" s="8" t="s">
         <v>4</v>
       </c>
@@ -5965,6 +6614,9 @@
       <c r="A22" t="s">
         <v>186</v>
       </c>
+      <c r="B22" t="s">
+        <v>467</v>
+      </c>
       <c r="C22" s="7" t="s">
         <v>4</v>
       </c>
@@ -5985,6 +6637,9 @@
       <c r="A23" t="s">
         <v>187</v>
       </c>
+      <c r="B23" t="s">
+        <v>468</v>
+      </c>
       <c r="C23" s="8" t="s">
         <v>4</v>
       </c>
@@ -6006,7 +6661,7 @@
         <v>188</v>
       </c>
       <c r="B24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C24" s="4">
         <v>4074.73</v>
@@ -6029,7 +6684,7 @@
         <v>189</v>
       </c>
       <c r="B25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C25" s="6">
         <v>2392.09</v>
@@ -6052,7 +6707,7 @@
         <v>190</v>
       </c>
       <c r="B26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C26" s="4">
         <v>2864.99</v>
@@ -6075,7 +6730,7 @@
         <v>191</v>
       </c>
       <c r="B27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C27" s="6">
         <v>40380.1</v>
@@ -6098,7 +6753,7 @@
         <v>192</v>
       </c>
       <c r="B28" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C28" s="4">
         <v>8029.87</v>
@@ -6117,14 +6772,14 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="A29" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6132,7 +6787,7 @@
         <v>193</v>
       </c>
       <c r="B30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C30" s="7">
         <v>102.08</v>
@@ -6155,7 +6810,7 @@
         <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C31" s="8">
         <v>3.6</v>
@@ -6178,7 +6833,7 @@
         <v>195</v>
       </c>
       <c r="B32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>4</v>
@@ -6200,6 +6855,9 @@
       <c r="A33" t="s">
         <v>196</v>
       </c>
+      <c r="B33" t="s">
+        <v>471</v>
+      </c>
       <c r="C33" s="8" t="s">
         <v>4</v>
       </c>
@@ -6221,7 +6879,7 @@
         <v>197</v>
       </c>
       <c r="B34" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>4</v>
@@ -6243,6 +6901,9 @@
       <c r="A35" t="s">
         <v>198</v>
       </c>
+      <c r="B35" t="s">
+        <v>504</v>
+      </c>
       <c r="C35" s="8" t="s">
         <v>4</v>
       </c>
@@ -6264,7 +6925,7 @@
         <v>199</v>
       </c>
       <c r="B36" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C36" s="7">
         <v>105.69</v>
@@ -6287,7 +6948,7 @@
         <v>200</v>
       </c>
       <c r="B37" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C37" s="6">
         <v>32393</v>
@@ -6310,7 +6971,7 @@
         <v>201</v>
       </c>
       <c r="B38" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>4</v>
@@ -6332,6 +6993,9 @@
       <c r="A39" t="s">
         <v>202</v>
       </c>
+      <c r="B39" t="s">
+        <v>452</v>
+      </c>
       <c r="C39" s="8" t="s">
         <v>4</v>
       </c>
@@ -6352,6 +7016,9 @@
       <c r="A40" t="s">
         <v>203</v>
       </c>
+      <c r="B40" t="s">
+        <v>454</v>
+      </c>
       <c r="C40" s="7" t="s">
         <v>4</v>
       </c>
@@ -6373,7 +7040,7 @@
         <v>204</v>
       </c>
       <c r="B41" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>4</v>
@@ -6395,6 +7062,9 @@
       <c r="A42" t="s">
         <v>205</v>
       </c>
+      <c r="B42" t="s">
+        <v>453</v>
+      </c>
       <c r="C42" s="7" t="s">
         <v>4</v>
       </c>
@@ -6416,7 +7086,7 @@
         <v>206</v>
       </c>
       <c r="B43" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C43" s="6">
         <v>32393</v>
@@ -6439,7 +7109,7 @@
         <v>207</v>
       </c>
       <c r="B44" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C44" s="4">
         <v>-32287.4</v>
@@ -6458,19 +7128,22 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
+      <c r="A45" s="19" t="s">
+        <v>503</v>
+      </c>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>209</v>
+        <v>208</v>
+      </c>
+      <c r="B46" t="s">
+        <v>444</v>
       </c>
       <c r="C46" s="4">
         <v>1212.5899999999999</v>
@@ -6490,7 +7163,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>210</v>
+        <v>209</v>
+      </c>
+      <c r="B47" t="s">
+        <v>455</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>4</v>
@@ -6510,7 +7186,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>211</v>
+        <v>210</v>
+      </c>
+      <c r="B48" t="s">
+        <v>445</v>
       </c>
       <c r="C48" s="4">
         <v>2400</v>
@@ -6530,7 +7209,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="B49" t="s">
+        <v>446</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>4</v>
@@ -6550,7 +7232,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="B50" t="s">
+        <v>447</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>4</v>
@@ -6570,7 +7255,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="B51" t="s">
+        <v>448</v>
       </c>
       <c r="C51" s="6">
         <v>3612.59</v>
@@ -6590,7 +7278,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="B52" t="s">
+        <v>449</v>
       </c>
       <c r="C52" s="4">
         <v>1360</v>
@@ -6610,7 +7301,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="B53" t="s">
+        <v>450</v>
       </c>
       <c r="C53" s="6">
         <v>2292.6999999999998</v>
@@ -6647,7 +7341,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>216</v>
+      </c>
+      <c r="B55" t="s">
+        <v>469</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>4</v>
@@ -6667,7 +7364,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>217</v>
+      </c>
+      <c r="B56" t="s">
+        <v>451</v>
       </c>
       <c r="C56" s="4">
         <v>3652.7</v>
@@ -6687,7 +7387,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>218</v>
+      </c>
+      <c r="B57" t="s">
+        <v>502</v>
       </c>
       <c r="C57" s="8">
         <v>-40.1</v>
@@ -6706,22 +7409,22 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
+      <c r="A58" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
       <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B59" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C59" s="6">
         <v>1276.2</v>
@@ -6741,10 +7444,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B60" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C60" s="4">
         <v>-23021.4</v>
@@ -6764,10 +7467,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B61" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C61" s="6">
         <v>53238.7</v>
@@ -6787,10 +7490,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B62" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C62" s="4">
         <v>30217.3</v>
@@ -6808,9 +7511,12 @@
         <v>51149.599999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>225</v>
+        <v>224</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>342</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>4</v>
@@ -6832,6 +7538,9 @@
       <c r="A64" t="s">
         <v>111</v>
       </c>
+      <c r="B64" t="s">
+        <v>472</v>
+      </c>
       <c r="C64" s="7" t="s">
         <v>4</v>
       </c>
@@ -6850,7 +7559,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="B65" t="s">
+        <v>473</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>4</v>
@@ -6870,7 +7582,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>470</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>4</v>
@@ -6890,7 +7605,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>228</v>
+        <v>227</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>474</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>4</v>
@@ -6910,7 +7628,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="B68" t="s">
+        <v>475</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>4</v>
@@ -6930,7 +7651,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>230</v>
+        <v>229</v>
+      </c>
+      <c r="B69" t="s">
+        <v>500</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>4</v>
@@ -6950,7 +7674,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>231</v>
+        <v>230</v>
+      </c>
+      <c r="B70" t="s">
+        <v>501</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>4</v>
@@ -6970,7 +7697,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+      <c r="B71" t="s">
+        <v>476</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>4</v>
@@ -6990,7 +7720,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>233</v>
+        <v>232</v>
+      </c>
+      <c r="B72" t="s">
+        <v>477</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>4</v>
@@ -7010,7 +7743,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>234</v>
+        <v>233</v>
+      </c>
+      <c r="B73" t="s">
+        <v>478</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>4</v>
@@ -7030,7 +7766,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>235</v>
+        <v>234</v>
+      </c>
+      <c r="B74" t="s">
+        <v>479</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>4</v>
@@ -7050,7 +7789,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>236</v>
+        <v>235</v>
+      </c>
+      <c r="B75" t="s">
+        <v>480</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>4</v>
@@ -7070,7 +7812,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+      <c r="B76" t="s">
+        <v>481</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>4</v>
@@ -7092,6 +7837,9 @@
       <c r="A77" t="s">
         <v>138</v>
       </c>
+      <c r="B77" t="s">
+        <v>482</v>
+      </c>
       <c r="C77" s="8" t="s">
         <v>4</v>
       </c>
@@ -7110,7 +7858,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="B78" t="s">
+        <v>483</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>4</v>
@@ -7130,7 +7881,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>239</v>
+        <v>238</v>
+      </c>
+      <c r="B79" t="s">
+        <v>484</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>4</v>
@@ -7150,7 +7904,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>240</v>
+        <v>239</v>
+      </c>
+      <c r="B80" t="s">
+        <v>485</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>4</v>
@@ -7170,7 +7927,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>241</v>
+        <v>240</v>
+      </c>
+      <c r="B81" t="s">
+        <v>486</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>4</v>
@@ -7190,7 +7950,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>242</v>
+        <v>241</v>
+      </c>
+      <c r="B82" t="s">
+        <v>487</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>4</v>
@@ -7210,7 +7973,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>243</v>
+        <v>242</v>
+      </c>
+      <c r="B83" t="s">
+        <v>488</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>4</v>
@@ -7230,7 +7996,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>244</v>
+        <v>243</v>
+      </c>
+      <c r="B84" t="s">
+        <v>489</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>4</v>
@@ -7250,7 +8019,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>245</v>
+        <v>244</v>
+      </c>
+      <c r="B85" t="s">
+        <v>490</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>4</v>
@@ -7270,7 +8042,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="B86" t="s">
+        <v>499</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>4</v>
@@ -7290,7 +8065,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>247</v>
+        <v>246</v>
+      </c>
+      <c r="B87" t="s">
+        <v>491</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>4</v>
@@ -7310,7 +8088,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>248</v>
+        <v>247</v>
+      </c>
+      <c r="B88" t="s">
+        <v>492</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>4</v>
@@ -7330,7 +8111,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>249</v>
+        <v>248</v>
+      </c>
+      <c r="B89" t="s">
+        <v>493</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>4</v>
@@ -7350,7 +8134,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="B90" t="s">
+        <v>494</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>4</v>
@@ -7370,7 +8157,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>251</v>
+        <v>250</v>
+      </c>
+      <c r="B91" t="s">
+        <v>495</v>
       </c>
       <c r="C91" s="6">
         <v>30217.3</v>
@@ -7390,7 +8180,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>252</v>
+        <v>251</v>
+      </c>
+      <c r="B92" t="s">
+        <v>496</v>
       </c>
       <c r="C92" s="4">
         <v>53238.7</v>
@@ -7410,7 +8203,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>253</v>
+        <v>252</v>
+      </c>
+      <c r="B93" t="s">
+        <v>497</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>4</v>
@@ -7430,7 +8226,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="B94" t="s">
+        <v>498</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>4</v>
@@ -7450,7 +8249,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="B95" t="s">
+        <v>366</v>
       </c>
       <c r="C95" s="6">
         <v>-23021.4</v>

</xml_diff>

<commit_message>
Add the column for account
</commit_message>
<xml_diff>
--- a/src/resource/balancesheet-sample.xlsx
+++ b/src/resource/balancesheet-sample.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BalanceSheet" sheetId="1" r:id="rId1"/>
     <sheet name="Incomentstatement" sheetId="2" r:id="rId2"/>
     <sheet name="Cashflowstatement" sheetId="3" r:id="rId3"/>
+    <sheet name="BS" sheetId="4" r:id="rId4"/>
+    <sheet name="IS" sheetId="5" r:id="rId5"/>
+    <sheet name="CS" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="593">
   <si>
     <t>流动资产</t>
   </si>
@@ -1069,9 +1072,6 @@
     <t>Minority interests</t>
   </si>
   <si>
-    <t>一、经营活动产生的现金流量Cash flow from operation activities</t>
-  </si>
-  <si>
     <t>Cash from sales of goods or rendering servicesies</t>
   </si>
   <si>
@@ -1099,9 +1099,6 @@
     <t>Net cash flow from operating activities</t>
   </si>
   <si>
-    <t>二、投资活动产生的现金流量：cash flows from investing activities</t>
-  </si>
-  <si>
     <t>Cash received from investments</t>
   </si>
   <si>
@@ -1546,9 +1543,6 @@
     <t>Net cash flow financing activities</t>
   </si>
   <si>
-    <t>三、筹资活动产生的现金流量：Cash flows from financing activities</t>
-  </si>
-  <si>
     <t>Received reduce and deposit cash pledge</t>
   </si>
   <si>
@@ -1556,13 +1550,280 @@
   </si>
   <si>
     <t>Other long-term investment</t>
+  </si>
+  <si>
+    <t>current assets</t>
+  </si>
+  <si>
+    <t>Non- current assets</t>
+  </si>
+  <si>
+    <t>Current liabilities</t>
+  </si>
+  <si>
+    <t>Non-current liabilities</t>
+  </si>
+  <si>
+    <t>Owner's equity (or equity)</t>
+  </si>
+  <si>
+    <t>营业总收入</t>
+  </si>
+  <si>
+    <t>营业总成本</t>
+  </si>
+  <si>
+    <t>营业利润</t>
+  </si>
+  <si>
+    <t>每股收益</t>
+  </si>
+  <si>
+    <t>其他综合收益</t>
+  </si>
+  <si>
+    <t>综合收益总额</t>
+  </si>
+  <si>
+    <t>一、经营活动产生的现金流量</t>
+  </si>
+  <si>
+    <t>Cash flow from operation activities</t>
+  </si>
+  <si>
+    <t>二、投资活动产生的现金流量：</t>
+  </si>
+  <si>
+    <t>cash flows from investing activities</t>
+  </si>
+  <si>
+    <t>三、筹资活动产生的现金流量：</t>
+  </si>
+  <si>
+    <t>Cash flows from financing activities</t>
+  </si>
+  <si>
+    <t>经营活动产生的现金流量</t>
+  </si>
+  <si>
+    <t>投资活动产生的现金流量</t>
+  </si>
+  <si>
+    <t>筹资活动产生的现金流量</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>settlementreverses</t>
+  </si>
+  <si>
+    <t>monetaryfunds</t>
+  </si>
+  <si>
+    <t>lending funds</t>
+  </si>
+  <si>
+    <t>lendingfunds</t>
+  </si>
+  <si>
+    <t>tranfinancialasset</t>
+  </si>
+  <si>
+    <t>derivfinancialasset</t>
+  </si>
+  <si>
+    <t>notesrecv</t>
+  </si>
+  <si>
+    <t>Advances to suppliers</t>
+  </si>
+  <si>
+    <t>premium receivable</t>
+  </si>
+  <si>
+    <t>accountsrecv</t>
+  </si>
+  <si>
+    <t>advancessupplier</t>
+  </si>
+  <si>
+    <t>premiumrecv</t>
+  </si>
+  <si>
+    <t>reinsurancerecv</t>
+  </si>
+  <si>
+    <t>reinsurancecontractres</t>
+  </si>
+  <si>
+    <t>interestrecv</t>
+  </si>
+  <si>
+    <t>dividendrecv</t>
+  </si>
+  <si>
+    <t>otherrecv</t>
+  </si>
+  <si>
+    <t>exportdrawbackrecv</t>
+  </si>
+  <si>
+    <t>subsidyrecv</t>
+  </si>
+  <si>
+    <t>cashdepositrecv</t>
+  </si>
+  <si>
+    <t>insiderrecv</t>
+  </si>
+  <si>
+    <t>fapur</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>dpexpense</t>
+  </si>
+  <si>
+    <t>currentassetlosssuspense</t>
+  </si>
+  <si>
+    <t>Due within one year of non-current assets</t>
+  </si>
+  <si>
+    <t>noncurrentasset1yr</t>
+  </si>
+  <si>
+    <t>othercurrentasset</t>
+  </si>
+  <si>
+    <t>subtotalcurrentasset</t>
+  </si>
+  <si>
+    <t>noncurrentasset</t>
+  </si>
+  <si>
+    <t>loanpayment</t>
+  </si>
+  <si>
+    <t>availsalefinancialasset</t>
+  </si>
+  <si>
+    <t>heldmaturityinv</t>
+  </si>
+  <si>
+    <t>ltaccountrecv</t>
+  </si>
+  <si>
+    <t>ltinv</t>
+  </si>
+  <si>
+    <t>otherltinv</t>
+  </si>
+  <si>
+    <t>invrealestate</t>
+  </si>
+  <si>
+    <t>fixedassetcost</t>
+  </si>
+  <si>
+    <t>accdepreciation</t>
+  </si>
+  <si>
+    <t>fixedassetnet</t>
+  </si>
+  <si>
+    <t>pifixedassets</t>
+  </si>
+  <si>
+    <t>Fixed assets net</t>
+  </si>
+  <si>
+    <t>constructioninprogress</t>
+  </si>
+  <si>
+    <t>engineermaterial</t>
+  </si>
+  <si>
+    <t>fixedassetliquid</t>
+  </si>
+  <si>
+    <t>prodbioasset</t>
+  </si>
+  <si>
+    <t>pubwelfarebioasset</t>
+  </si>
+  <si>
+    <t>oidgasasset</t>
+  </si>
+  <si>
+    <t>intangibleasset</t>
+  </si>
+  <si>
+    <t>devexpend</t>
+  </si>
+  <si>
+    <t>goodwill</t>
+  </si>
+  <si>
+    <t>ltprepaidexpense</t>
+  </si>
+  <si>
+    <t>rightsharecirculation</t>
+  </si>
+  <si>
+    <t>defincometaxasset</t>
+  </si>
+  <si>
+    <t>othernoncurrentasset</t>
+  </si>
+  <si>
+    <t>subtotalnoncurrentasset</t>
+  </si>
+  <si>
+    <t>totalasset</t>
+  </si>
+  <si>
+    <t>currentliability</t>
+  </si>
+  <si>
+    <t>stloan</t>
+  </si>
+  <si>
+    <t>borrowcentralbank</t>
+  </si>
+  <si>
+    <t>depositcustominterbank</t>
+  </si>
+  <si>
+    <t>depositfund</t>
+  </si>
+  <si>
+    <t>tranfinancialliability</t>
+  </si>
+  <si>
+    <t>derivfinancialliability</t>
+  </si>
+  <si>
+    <t>notespay</t>
+  </si>
+  <si>
+    <t>accountpay</t>
+  </si>
+  <si>
+    <t>advancepay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1623,6 +1884,14 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1666,7 +1935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1712,12 +1981,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1732,6 +1995,19 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2036,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B114" sqref="A3:C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,18 +2370,18 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="19" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2229,7 +2505,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -2461,7 +2737,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -2490,7 +2766,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -2519,7 +2795,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -2548,7 +2824,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2577,7 +2853,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C20">
         <v>116362</v>
@@ -2606,7 +2882,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -2693,7 +2969,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2722,7 +2998,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -2834,18 +3110,18 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="19" t="s">
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2853,7 +3129,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -2998,7 +3274,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -3172,7 +3448,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C41">
         <v>48155.4</v>
@@ -3317,7 +3593,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -3491,7 +3767,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
@@ -3549,7 +3825,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C54">
         <v>431905</v>
@@ -3632,18 +3908,18 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="19" t="s">
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3680,7 +3956,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
@@ -3709,7 +3985,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -3738,7 +4014,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
@@ -3796,7 +4072,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
@@ -3912,7 +4188,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C67">
         <v>230044</v>
@@ -3941,7 +4217,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C68" t="s">
         <v>4</v>
@@ -4028,7 +4304,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C71">
         <v>5224.08</v>
@@ -4115,7 +4391,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
@@ -4144,7 +4420,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C75" t="s">
         <v>4</v>
@@ -4202,7 +4478,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C77" t="s">
         <v>4</v>
@@ -4231,7 +4507,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C78" t="s">
         <v>4</v>
@@ -4260,7 +4536,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C79" t="s">
         <v>4</v>
@@ -4288,8 +4564,8 @@
       <c r="A80" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="21" t="s">
-        <v>394</v>
+      <c r="B80" s="19" t="s">
+        <v>392</v>
       </c>
       <c r="C80" t="s">
         <v>4</v>
@@ -4318,7 +4594,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C81">
         <v>4182670</v>
@@ -4347,7 +4623,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C82">
         <v>3057.07</v>
@@ -4376,7 +4652,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C83" t="s">
         <v>4</v>
@@ -4405,7 +4681,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C84" t="s">
         <v>4</v>
@@ -4463,7 +4739,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C86" t="s">
         <v>4</v>
@@ -4575,18 +4851,18 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
+      <c r="A90" s="24" t="s">
         <v>310</v>
       </c>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="17" t="s">
+      <c r="B90" s="25"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="18"/>
+      <c r="E90" s="25"/>
+      <c r="F90" s="25"/>
+      <c r="G90" s="25"/>
+      <c r="H90" s="25"/>
       <c r="I90" s="1"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -4768,7 +5044,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C97" s="6">
         <v>195883</v>
@@ -4851,18 +5127,18 @@
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="17" t="s">
+      <c r="A100" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="B100" s="18"/>
-      <c r="C100" s="18"/>
-      <c r="D100" s="17" t="s">
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="E100" s="18"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="18"/>
-      <c r="H100" s="18"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="25"/>
+      <c r="H100" s="25"/>
       <c r="I100" s="1"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4928,7 +5204,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>4</v>
@@ -4957,7 +5233,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>4</v>
@@ -5015,7 +5291,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C106" s="4">
         <v>52697.3</v>
@@ -5044,7 +5320,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>4</v>
@@ -5102,7 +5378,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>4</v>
@@ -5130,8 +5406,8 @@
       <c r="A110" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="21" t="s">
-        <v>406</v>
+      <c r="B110" s="19" t="s">
+        <v>404</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>4</v>
@@ -5159,8 +5435,8 @@
       <c r="A111" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="21" t="s">
-        <v>407</v>
+      <c r="B111" s="19" t="s">
+        <v>405</v>
       </c>
       <c r="C111" s="6">
         <v>1249190</v>
@@ -5189,7 +5465,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C112" s="4">
         <v>137397</v>
@@ -5508,8 +5784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5542,7 +5818,7 @@
         <v>116</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C3" s="6">
         <v>39451.800000000003</v>
@@ -5558,16 +5834,16 @@
       <c r="C4" s="4">
         <v>39451.800000000003</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>410</v>
+      <c r="E4" s="20" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>411</v>
+      <c r="B5" s="19" t="s">
+        <v>409</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>4</v>
@@ -5578,7 +5854,7 @@
         <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>4</v>
@@ -5588,8 +5864,8 @@
       <c r="A7" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>413</v>
+      <c r="B7" s="19" t="s">
+        <v>411</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>4</v>
@@ -5600,7 +5876,7 @@
         <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>4</v>
@@ -5622,7 +5898,7 @@
         <v>123</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C10" s="4">
         <v>37868.800000000003</v>
@@ -5655,7 +5931,7 @@
         <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>4</v>
@@ -5666,7 +5942,7 @@
         <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>4</v>
@@ -5687,8 +5963,8 @@
       <c r="A16" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>418</v>
+      <c r="B16" s="19" t="s">
+        <v>416</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>4</v>
@@ -5699,7 +5975,7 @@
         <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>4</v>
@@ -5710,7 +5986,7 @@
         <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>4</v>
@@ -5720,8 +5996,8 @@
       <c r="A19" t="s">
         <v>132</v>
       </c>
-      <c r="B19" s="21" t="s">
-        <v>421</v>
+      <c r="B19" s="19" t="s">
+        <v>419</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>4</v>
@@ -5731,8 +6007,8 @@
       <c r="A20" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="21" t="s">
-        <v>422</v>
+      <c r="B20" s="19" t="s">
+        <v>420</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>4</v>
@@ -5764,8 +6040,8 @@
       <c r="A23" t="s">
         <v>136</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>423</v>
+      <c r="B23" s="19" t="s">
+        <v>421</v>
       </c>
       <c r="C23" s="6">
         <v>2210.62</v>
@@ -5808,8 +6084,8 @@
       <c r="A27" t="s">
         <v>140</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>424</v>
+      <c r="B27" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>4</v>
@@ -5819,8 +6095,8 @@
       <c r="A28" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="21" t="s">
-        <v>425</v>
+      <c r="B28" s="19" t="s">
+        <v>423</v>
       </c>
       <c r="C28" s="7">
         <v>618.82000000000005</v>
@@ -5830,8 +6106,8 @@
       <c r="A29" t="s">
         <v>142</v>
       </c>
-      <c r="B29" s="21" t="s">
-        <v>426</v>
+      <c r="B29" s="19" t="s">
+        <v>424</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>4</v>
@@ -5841,8 +6117,8 @@
       <c r="A30" t="s">
         <v>143</v>
       </c>
-      <c r="B30" s="21" t="s">
-        <v>427</v>
+      <c r="B30" s="19" t="s">
+        <v>425</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>4</v>
@@ -5852,8 +6128,8 @@
       <c r="A31" t="s">
         <v>144</v>
       </c>
-      <c r="B31" s="21" t="s">
-        <v>428</v>
+      <c r="B31" s="19" t="s">
+        <v>426</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>4</v>
@@ -5863,8 +6139,8 @@
       <c r="A32" t="s">
         <v>145</v>
       </c>
-      <c r="B32" s="21" t="s">
-        <v>429</v>
+      <c r="B32" s="19" t="s">
+        <v>427</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>4</v>
@@ -5874,8 +6150,8 @@
       <c r="A33" t="s">
         <v>146</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>430</v>
+      <c r="B33" s="19" t="s">
+        <v>428</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>4</v>
@@ -5885,8 +6161,8 @@
       <c r="A34" t="s">
         <v>147</v>
       </c>
-      <c r="B34" s="21" t="s">
-        <v>431</v>
+      <c r="B34" s="19" t="s">
+        <v>429</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>4</v>
@@ -5929,8 +6205,8 @@
       <c r="A38" t="s">
         <v>151</v>
       </c>
-      <c r="B38" s="21" t="s">
-        <v>432</v>
+      <c r="B38" s="19" t="s">
+        <v>430</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>4</v>
@@ -5963,7 +6239,7 @@
         <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>4</v>
@@ -5985,7 +6261,7 @@
         <v>156</v>
       </c>
       <c r="B43" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C43" s="6">
         <v>2141.65</v>
@@ -6007,7 +6283,7 @@
         <v>158</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C45" s="1"/>
     </row>
@@ -6016,7 +6292,7 @@
         <v>159</v>
       </c>
       <c r="B46" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>160</v>
@@ -6027,7 +6303,7 @@
         <v>161</v>
       </c>
       <c r="B47" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>160</v>
@@ -6038,7 +6314,7 @@
         <v>162</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C48" s="7">
         <v>-439.5</v>
@@ -6049,7 +6325,7 @@
         <v>163</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C49" s="6">
         <v>1781.81</v>
@@ -6060,7 +6336,7 @@
         <v>164</v>
       </c>
       <c r="B50" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C50" s="4">
         <v>1702.15</v>
@@ -6070,8 +6346,8 @@
       <c r="A51" t="s">
         <v>165</v>
       </c>
-      <c r="B51" s="21" t="s">
-        <v>441</v>
+      <c r="B51" s="19" t="s">
+        <v>439</v>
       </c>
       <c r="C51" s="8">
         <v>79.66</v>
@@ -6138,8 +6414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6185,15 +6461,17 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>344</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+    <row r="3" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6201,7 +6479,7 @@
         <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C4" s="4">
         <v>48245.5</v>
@@ -6224,7 +6502,7 @@
         <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>4</v>
@@ -6247,7 +6525,7 @@
         <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
@@ -6270,7 +6548,7 @@
         <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>4</v>
@@ -6293,7 +6571,7 @@
         <v>172</v>
       </c>
       <c r="B8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -6316,7 +6594,7 @@
         <v>173</v>
       </c>
       <c r="B9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>4</v>
@@ -6339,7 +6617,7 @@
         <v>174</v>
       </c>
       <c r="B10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>4</v>
@@ -6362,7 +6640,7 @@
         <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>4</v>
@@ -6385,7 +6663,7 @@
         <v>176</v>
       </c>
       <c r="B12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>4</v>
@@ -6407,8 +6685,8 @@
       <c r="A13" t="s">
         <v>177</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>456</v>
+      <c r="B13" s="21" t="s">
+        <v>454</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>4</v>
@@ -6431,7 +6709,7 @@
         <v>178</v>
       </c>
       <c r="B14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>4</v>
@@ -6453,8 +6731,8 @@
       <c r="A15" t="s">
         <v>179</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>460</v>
+      <c r="B15" s="22" t="s">
+        <v>458</v>
       </c>
       <c r="C15" s="8">
         <v>48.65</v>
@@ -6477,7 +6755,7 @@
         <v>180</v>
       </c>
       <c r="B16" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C16" s="7">
         <v>115.85</v>
@@ -6500,7 +6778,7 @@
         <v>181</v>
       </c>
       <c r="B17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C17" s="6">
         <v>48410</v>
@@ -6523,7 +6801,7 @@
         <v>182</v>
       </c>
       <c r="B18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C18" s="4">
         <v>31048.3</v>
@@ -6546,7 +6824,7 @@
         <v>183</v>
       </c>
       <c r="B19" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>4</v>
@@ -6569,7 +6847,7 @@
         <v>184</v>
       </c>
       <c r="B20" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>4</v>
@@ -6592,7 +6870,7 @@
         <v>185</v>
       </c>
       <c r="B21" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>4</v>
@@ -6615,7 +6893,7 @@
         <v>186</v>
       </c>
       <c r="B22" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>4</v>
@@ -6638,7 +6916,7 @@
         <v>187</v>
       </c>
       <c r="B23" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>4</v>
@@ -6661,7 +6939,7 @@
         <v>188</v>
       </c>
       <c r="B24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C24" s="4">
         <v>4074.73</v>
@@ -6684,7 +6962,7 @@
         <v>189</v>
       </c>
       <c r="B25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C25" s="6">
         <v>2392.09</v>
@@ -6707,7 +6985,7 @@
         <v>190</v>
       </c>
       <c r="B26" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C26" s="4">
         <v>2864.99</v>
@@ -6730,7 +7008,7 @@
         <v>191</v>
       </c>
       <c r="B27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C27" s="6">
         <v>40380.1</v>
@@ -6753,7 +7031,7 @@
         <v>192</v>
       </c>
       <c r="B28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C28" s="4">
         <v>8029.87</v>
@@ -6771,15 +7049,17 @@
         <v>-9719.7199999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>354</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>518</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6787,7 +7067,7 @@
         <v>193</v>
       </c>
       <c r="B30" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C30" s="7">
         <v>102.08</v>
@@ -6810,7 +7090,7 @@
         <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C31" s="8">
         <v>3.6</v>
@@ -6833,7 +7113,7 @@
         <v>195</v>
       </c>
       <c r="B32" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>4</v>
@@ -6856,7 +7136,7 @@
         <v>196</v>
       </c>
       <c r="B33" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>4</v>
@@ -6879,7 +7159,7 @@
         <v>197</v>
       </c>
       <c r="B34" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>4</v>
@@ -6902,7 +7182,7 @@
         <v>198</v>
       </c>
       <c r="B35" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>4</v>
@@ -6925,7 +7205,7 @@
         <v>199</v>
       </c>
       <c r="B36" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C36" s="7">
         <v>105.69</v>
@@ -6948,7 +7228,7 @@
         <v>200</v>
       </c>
       <c r="B37" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C37" s="6">
         <v>32393</v>
@@ -6971,7 +7251,7 @@
         <v>201</v>
       </c>
       <c r="B38" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>4</v>
@@ -6994,7 +7274,7 @@
         <v>202</v>
       </c>
       <c r="B39" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>4</v>
@@ -7017,7 +7297,7 @@
         <v>203</v>
       </c>
       <c r="B40" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>4</v>
@@ -7040,7 +7320,7 @@
         <v>204</v>
       </c>
       <c r="B41" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>4</v>
@@ -7063,7 +7343,7 @@
         <v>205</v>
       </c>
       <c r="B42" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>4</v>
@@ -7086,7 +7366,7 @@
         <v>206</v>
       </c>
       <c r="B43" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C43" s="6">
         <v>32393</v>
@@ -7109,7 +7389,7 @@
         <v>207</v>
       </c>
       <c r="B44" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C44" s="4">
         <v>-32287.4</v>
@@ -7127,15 +7407,17 @@
         <v>-5152.84</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
-        <v>503</v>
-      </c>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
+        <v>519</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>520</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -7143,7 +7425,7 @@
         <v>208</v>
       </c>
       <c r="B46" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C46" s="4">
         <v>1212.5899999999999</v>
@@ -7166,7 +7448,7 @@
         <v>209</v>
       </c>
       <c r="B47" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>4</v>
@@ -7189,7 +7471,7 @@
         <v>210</v>
       </c>
       <c r="B48" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C48" s="4">
         <v>2400</v>
@@ -7212,7 +7494,7 @@
         <v>211</v>
       </c>
       <c r="B49" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>4</v>
@@ -7235,7 +7517,7 @@
         <v>212</v>
       </c>
       <c r="B50" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>4</v>
@@ -7258,7 +7540,7 @@
         <v>213</v>
       </c>
       <c r="B51" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C51" s="6">
         <v>3612.59</v>
@@ -7281,7 +7563,7 @@
         <v>214</v>
       </c>
       <c r="B52" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C52" s="4">
         <v>1360</v>
@@ -7304,7 +7586,7 @@
         <v>215</v>
       </c>
       <c r="B53" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C53" s="6">
         <v>2292.6999999999998</v>
@@ -7344,7 +7626,7 @@
         <v>216</v>
       </c>
       <c r="B55" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>4</v>
@@ -7367,7 +7649,7 @@
         <v>217</v>
       </c>
       <c r="B56" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C56" s="4">
         <v>3652.7</v>
@@ -7390,7 +7672,7 @@
         <v>218</v>
       </c>
       <c r="B57" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C57" s="8">
         <v>-40.1</v>
@@ -7424,7 +7706,7 @@
         <v>220</v>
       </c>
       <c r="B59" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C59" s="6">
         <v>1276.2</v>
@@ -7447,7 +7729,7 @@
         <v>221</v>
       </c>
       <c r="B60" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C60" s="4">
         <v>-23021.4</v>
@@ -7470,7 +7752,7 @@
         <v>222</v>
       </c>
       <c r="B61" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C61" s="6">
         <v>53238.7</v>
@@ -7493,7 +7775,7 @@
         <v>223</v>
       </c>
       <c r="B62" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C62" s="4">
         <v>30217.3</v>
@@ -7515,7 +7797,7 @@
       <c r="A63" t="s">
         <v>224</v>
       </c>
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="22" t="s">
         <v>342</v>
       </c>
       <c r="C63" s="8" t="s">
@@ -7539,7 +7821,7 @@
         <v>111</v>
       </c>
       <c r="B64" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>4</v>
@@ -7562,7 +7844,7 @@
         <v>225</v>
       </c>
       <c r="B65" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>4</v>
@@ -7584,8 +7866,8 @@
       <c r="A66" t="s">
         <v>226</v>
       </c>
-      <c r="B66" s="23" t="s">
-        <v>470</v>
+      <c r="B66" s="21" t="s">
+        <v>468</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>4</v>
@@ -7607,8 +7889,8 @@
       <c r="A67" t="s">
         <v>227</v>
       </c>
-      <c r="B67" s="23" t="s">
-        <v>474</v>
+      <c r="B67" s="21" t="s">
+        <v>472</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>4</v>
@@ -7631,7 +7913,7 @@
         <v>228</v>
       </c>
       <c r="B68" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>4</v>
@@ -7654,7 +7936,7 @@
         <v>229</v>
       </c>
       <c r="B69" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>4</v>
@@ -7677,7 +7959,7 @@
         <v>230</v>
       </c>
       <c r="B70" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>4</v>
@@ -7700,7 +7982,7 @@
         <v>231</v>
       </c>
       <c r="B71" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>4</v>
@@ -7723,7 +8005,7 @@
         <v>232</v>
       </c>
       <c r="B72" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>4</v>
@@ -7746,7 +8028,7 @@
         <v>233</v>
       </c>
       <c r="B73" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>4</v>
@@ -7769,7 +8051,7 @@
         <v>234</v>
       </c>
       <c r="B74" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>4</v>
@@ -7792,7 +8074,7 @@
         <v>235</v>
       </c>
       <c r="B75" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>4</v>
@@ -7815,7 +8097,7 @@
         <v>236</v>
       </c>
       <c r="B76" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>4</v>
@@ -7838,7 +8120,7 @@
         <v>138</v>
       </c>
       <c r="B77" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>4</v>
@@ -7861,7 +8143,7 @@
         <v>237</v>
       </c>
       <c r="B78" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>4</v>
@@ -7884,7 +8166,7 @@
         <v>238</v>
       </c>
       <c r="B79" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>4</v>
@@ -7907,7 +8189,7 @@
         <v>239</v>
       </c>
       <c r="B80" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>4</v>
@@ -7930,7 +8212,7 @@
         <v>240</v>
       </c>
       <c r="B81" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>4</v>
@@ -7953,7 +8235,7 @@
         <v>241</v>
       </c>
       <c r="B82" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>4</v>
@@ -7976,7 +8258,7 @@
         <v>242</v>
       </c>
       <c r="B83" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>4</v>
@@ -7999,7 +8281,7 @@
         <v>243</v>
       </c>
       <c r="B84" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>4</v>
@@ -8022,7 +8304,7 @@
         <v>244</v>
       </c>
       <c r="B85" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>4</v>
@@ -8045,7 +8327,7 @@
         <v>245</v>
       </c>
       <c r="B86" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>4</v>
@@ -8068,7 +8350,7 @@
         <v>246</v>
       </c>
       <c r="B87" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>4</v>
@@ -8091,7 +8373,7 @@
         <v>247</v>
       </c>
       <c r="B88" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>4</v>
@@ -8114,7 +8396,7 @@
         <v>248</v>
       </c>
       <c r="B89" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>4</v>
@@ -8137,7 +8419,7 @@
         <v>249</v>
       </c>
       <c r="B90" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>4</v>
@@ -8160,7 +8442,7 @@
         <v>250</v>
       </c>
       <c r="B91" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C91" s="6">
         <v>30217.3</v>
@@ -8183,7 +8465,7 @@
         <v>251</v>
       </c>
       <c r="B92" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C92" s="4">
         <v>53238.7</v>
@@ -8206,7 +8488,7 @@
         <v>252</v>
       </c>
       <c r="B93" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>4</v>
@@ -8229,7 +8511,7 @@
         <v>253</v>
       </c>
       <c r="B94" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>4</v>
@@ -8252,7 +8534,7 @@
         <v>254</v>
       </c>
       <c r="B95" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C95" s="6">
         <v>-23021.4</v>
@@ -8271,12 +8553,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A58:F58"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst1"/>
     <hyperlink ref="A5" r:id="rId2" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst75"/>
@@ -8370,4 +8646,2477 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>504</v>
+      </c>
+      <c r="C1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>528</v>
+      </c>
+      <c r="C4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>367</v>
+      </c>
+      <c r="C6" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>533</v>
+      </c>
+      <c r="C9" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>534</v>
+      </c>
+      <c r="C10" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>264</v>
+      </c>
+      <c r="C11" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C12" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>368</v>
+      </c>
+      <c r="C14" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>369</v>
+      </c>
+      <c r="C15" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>370</v>
+      </c>
+      <c r="C16" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>371</v>
+      </c>
+      <c r="C17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>372</v>
+      </c>
+      <c r="C18" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>373</v>
+      </c>
+      <c r="C19" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>267</v>
+      </c>
+      <c r="C20" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>270</v>
+      </c>
+      <c r="C21" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>374</v>
+      </c>
+      <c r="C22" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>375</v>
+      </c>
+      <c r="C23" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>551</v>
+      </c>
+      <c r="C24" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>271</v>
+      </c>
+      <c r="C25" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>272</v>
+      </c>
+      <c r="C26" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>505</v>
+      </c>
+      <c r="C27" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>376</v>
+      </c>
+      <c r="C28" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>274</v>
+      </c>
+      <c r="C29" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>275</v>
+      </c>
+      <c r="C30" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>276</v>
+      </c>
+      <c r="C31" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C32" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>503</v>
+      </c>
+      <c r="C33" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>278</v>
+      </c>
+      <c r="C34" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>279</v>
+      </c>
+      <c r="C35" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>280</v>
+      </c>
+      <c r="C36" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>281</v>
+      </c>
+      <c r="C37" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>282</v>
+      </c>
+      <c r="C38" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>567</v>
+      </c>
+      <c r="C39" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>283</v>
+      </c>
+      <c r="C40" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>284</v>
+      </c>
+      <c r="C41" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>285</v>
+      </c>
+      <c r="C42" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>286</v>
+      </c>
+      <c r="C43" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>378</v>
+      </c>
+      <c r="C44" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>290</v>
+      </c>
+      <c r="C45" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>289</v>
+      </c>
+      <c r="C46" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>288</v>
+      </c>
+      <c r="C47" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>287</v>
+      </c>
+      <c r="C48" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>292</v>
+      </c>
+      <c r="B49" t="s">
+        <v>291</v>
+      </c>
+      <c r="C49" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>379</v>
+      </c>
+      <c r="C50" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>293</v>
+      </c>
+      <c r="C51" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>502</v>
+      </c>
+      <c r="C52" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>294</v>
+      </c>
+      <c r="C53" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>295</v>
+      </c>
+      <c r="C54" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>506</v>
+      </c>
+      <c r="C55" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" t="s">
+        <v>297</v>
+      </c>
+      <c r="C56" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
+        <v>380</v>
+      </c>
+      <c r="C57" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
+        <v>381</v>
+      </c>
+      <c r="C58" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>382</v>
+      </c>
+      <c r="C59" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" t="s">
+        <v>262</v>
+      </c>
+      <c r="C60" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" t="s">
+        <v>383</v>
+      </c>
+      <c r="C61" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" t="s">
+        <v>298</v>
+      </c>
+      <c r="C62" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" t="s">
+        <v>299</v>
+      </c>
+      <c r="C63" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" t="s">
+        <v>300</v>
+      </c>
+      <c r="C64" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>302</v>
+      </c>
+      <c r="B67" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>304</v>
+      </c>
+      <c r="B68" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="19" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" s="23" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B98" s="23" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>102</v>
+      </c>
+      <c r="B101" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>103</v>
+      </c>
+      <c r="B102" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>105</v>
+      </c>
+      <c r="B104" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>107</v>
+      </c>
+      <c r="B106" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>109</v>
+      </c>
+      <c r="B108" s="19" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>110</v>
+      </c>
+      <c r="B109" s="19" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>111</v>
+      </c>
+      <c r="B110" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>113</v>
+      </c>
+      <c r="B112" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet1"/>
+    <hyperlink ref="A3" r:id="rId2" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet123"/>
+    <hyperlink ref="A4" r:id="rId3" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet124"/>
+    <hyperlink ref="A5" r:id="rId4" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet110"/>
+    <hyperlink ref="A6" r:id="rId5" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet143"/>
+    <hyperlink ref="A7" r:id="rId6" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet4"/>
+    <hyperlink ref="A8" r:id="rId7" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet7"/>
+    <hyperlink ref="A9" r:id="rId8" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet11"/>
+    <hyperlink ref="A10" r:id="rId9" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet125"/>
+    <hyperlink ref="A11" r:id="rId10" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet126"/>
+    <hyperlink ref="A12" r:id="rId11" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet127"/>
+    <hyperlink ref="A13" r:id="rId12" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet6"/>
+    <hyperlink ref="A14" r:id="rId13" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet5"/>
+    <hyperlink ref="A15" r:id="rId14" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet8"/>
+    <hyperlink ref="A16" r:id="rId15" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet65"/>
+    <hyperlink ref="A17" r:id="rId16" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet12"/>
+    <hyperlink ref="A18" r:id="rId17" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet144"/>
+    <hyperlink ref="A19" r:id="rId18" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet13"/>
+    <hyperlink ref="A20" r:id="rId19" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet128"/>
+    <hyperlink ref="A21" r:id="rId20" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet14"/>
+    <hyperlink ref="A22" r:id="rId21" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet129"/>
+    <hyperlink ref="A23" r:id="rId22" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet18"/>
+    <hyperlink ref="A24" r:id="rId23" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet19"/>
+    <hyperlink ref="A25" r:id="rId24" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet20"/>
+    <hyperlink ref="A26" r:id="rId25" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet21"/>
+    <hyperlink ref="A28" r:id="rId26" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet130"/>
+    <hyperlink ref="A29" r:id="rId27" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet111"/>
+    <hyperlink ref="A30" r:id="rId28" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet112"/>
+    <hyperlink ref="A31" r:id="rId29" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet42"/>
+    <hyperlink ref="A32" r:id="rId30" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet22"/>
+    <hyperlink ref="A33" r:id="rId31" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet24"/>
+    <hyperlink ref="A34" r:id="rId32" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet113"/>
+    <hyperlink ref="A35" r:id="rId33" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet29"/>
+    <hyperlink ref="A36" r:id="rId34" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet30"/>
+    <hyperlink ref="A37" r:id="rId35" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet31"/>
+    <hyperlink ref="A38" r:id="rId36" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet32"/>
+    <hyperlink ref="A39" r:id="rId37" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet105"/>
+    <hyperlink ref="A40" r:id="rId38" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet34"/>
+    <hyperlink ref="A41" r:id="rId39" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet33"/>
+    <hyperlink ref="A42" r:id="rId40" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet35"/>
+    <hyperlink ref="A43" r:id="rId41" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet114"/>
+    <hyperlink ref="A44" r:id="rId42" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet145"/>
+    <hyperlink ref="A45" r:id="rId43" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet115"/>
+    <hyperlink ref="A46" r:id="rId44" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet38"/>
+    <hyperlink ref="A47" r:id="rId45" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet116"/>
+    <hyperlink ref="A48" r:id="rId46" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet117"/>
+    <hyperlink ref="A49" r:id="rId47" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet40"/>
+    <hyperlink ref="A50" r:id="rId48" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet146"/>
+    <hyperlink ref="A51" r:id="rId49" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet44"/>
+    <hyperlink ref="A52" r:id="rId50" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet41"/>
+    <hyperlink ref="A53" r:id="rId51" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet118"/>
+    <hyperlink ref="A54" r:id="rId52" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet46"/>
+    <hyperlink ref="A56" r:id="rId53" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet47"/>
+    <hyperlink ref="A57" r:id="rId54" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet131"/>
+    <hyperlink ref="A58" r:id="rId55" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet132"/>
+    <hyperlink ref="A59" r:id="rId56" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet133"/>
+    <hyperlink ref="A60" r:id="rId57" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet119"/>
+    <hyperlink ref="A61" r:id="rId58" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet147"/>
+    <hyperlink ref="A62" r:id="rId59" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet48"/>
+    <hyperlink ref="A63" r:id="rId60" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet49"/>
+    <hyperlink ref="A64" r:id="rId61" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet50"/>
+    <hyperlink ref="A65" r:id="rId62" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet134"/>
+    <hyperlink ref="A66" r:id="rId63" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet135"/>
+    <hyperlink ref="A67" r:id="rId64" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet52"/>
+    <hyperlink ref="A68" r:id="rId65" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet55"/>
+    <hyperlink ref="A69" r:id="rId66" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet109"/>
+    <hyperlink ref="A70" r:id="rId67" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet54"/>
+    <hyperlink ref="A71" r:id="rId68" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet56"/>
+    <hyperlink ref="A72" r:id="rId69" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet148"/>
+    <hyperlink ref="A73" r:id="rId70" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet58"/>
+    <hyperlink ref="A74" r:id="rId71" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet57"/>
+    <hyperlink ref="A75" r:id="rId72" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet136"/>
+    <hyperlink ref="A76" r:id="rId73" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet61"/>
+    <hyperlink ref="A77" r:id="rId74" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet137"/>
+    <hyperlink ref="A78" r:id="rId75" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet138"/>
+    <hyperlink ref="A79" r:id="rId76" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet139"/>
+    <hyperlink ref="A80" r:id="rId77" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet140"/>
+    <hyperlink ref="A81" r:id="rId78" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet149"/>
+    <hyperlink ref="A82" r:id="rId79" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet150"/>
+    <hyperlink ref="A83" r:id="rId80" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet73"/>
+    <hyperlink ref="A84" r:id="rId81" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet64"/>
+    <hyperlink ref="A85" r:id="rId82" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet62"/>
+    <hyperlink ref="A86" r:id="rId83" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet63"/>
+    <hyperlink ref="A87" r:id="rId84" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet66"/>
+    <hyperlink ref="A89" r:id="rId85" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet67"/>
+    <hyperlink ref="A90" r:id="rId86" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet68"/>
+    <hyperlink ref="A91" r:id="rId87" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet69"/>
+    <hyperlink ref="A92" r:id="rId88" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet74"/>
+    <hyperlink ref="A93" r:id="rId89" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet120"/>
+    <hyperlink ref="A94" r:id="rId90" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet76"/>
+    <hyperlink ref="A95" r:id="rId91" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet70"/>
+    <hyperlink ref="A96" r:id="rId92" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet75"/>
+    <hyperlink ref="A97" r:id="rId93" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet77"/>
+    <hyperlink ref="A99" r:id="rId94" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet80"/>
+    <hyperlink ref="A100" r:id="rId95" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet81"/>
+    <hyperlink ref="A101" r:id="rId96" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet121"/>
+    <hyperlink ref="A102" r:id="rId97" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet151"/>
+    <hyperlink ref="A103" r:id="rId98" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet82"/>
+    <hyperlink ref="A104" r:id="rId99" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet141"/>
+    <hyperlink ref="A105" r:id="rId100" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet88"/>
+    <hyperlink ref="A106" r:id="rId101" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet84"/>
+    <hyperlink ref="A107" r:id="rId102" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet108"/>
+    <hyperlink ref="A108" r:id="rId103" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet142"/>
+    <hyperlink ref="A109" r:id="rId104" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet122"/>
+    <hyperlink ref="A110" r:id="rId105" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet79"/>
+    <hyperlink ref="A111" r:id="rId106" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet86"/>
+    <hyperlink ref="A112" r:id="rId107" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=600030&amp;type=cbsheet87"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId108"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>509</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>510</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>512</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>514</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>439</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B92"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>521</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>522</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>193</v>
+      </c>
+      <c r="B28" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>194</v>
+      </c>
+      <c r="B29" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>195</v>
+      </c>
+      <c r="B30" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B32" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B33" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>203</v>
+      </c>
+      <c r="B38" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>207</v>
+      </c>
+      <c r="B42" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>523</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>208</v>
+      </c>
+      <c r="B44" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>209</v>
+      </c>
+      <c r="B45" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>210</v>
+      </c>
+      <c r="B46" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>215</v>
+      </c>
+      <c r="B51" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>216</v>
+      </c>
+      <c r="B52" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>217</v>
+      </c>
+      <c r="B53" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>218</v>
+      </c>
+      <c r="B54" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>220</v>
+      </c>
+      <c r="B56" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>221</v>
+      </c>
+      <c r="B57" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>224</v>
+      </c>
+      <c r="B60" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>225</v>
+      </c>
+      <c r="B62" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>226</v>
+      </c>
+      <c r="B63" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>227</v>
+      </c>
+      <c r="B64" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>228</v>
+      </c>
+      <c r="B65" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>229</v>
+      </c>
+      <c r="B66" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>230</v>
+      </c>
+      <c r="B67" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>231</v>
+      </c>
+      <c r="B68" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>232</v>
+      </c>
+      <c r="B69" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>233</v>
+      </c>
+      <c r="B70" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>234</v>
+      </c>
+      <c r="B71" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>235</v>
+      </c>
+      <c r="B72" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>236</v>
+      </c>
+      <c r="B73" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>138</v>
+      </c>
+      <c r="B74" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>238</v>
+      </c>
+      <c r="B76" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>239</v>
+      </c>
+      <c r="B77" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>240</v>
+      </c>
+      <c r="B78" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>241</v>
+      </c>
+      <c r="B79" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>242</v>
+      </c>
+      <c r="B80" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>243</v>
+      </c>
+      <c r="B81" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>244</v>
+      </c>
+      <c r="B82" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>245</v>
+      </c>
+      <c r="B83" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>246</v>
+      </c>
+      <c r="B84" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>247</v>
+      </c>
+      <c r="B85" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>248</v>
+      </c>
+      <c r="B86" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>249</v>
+      </c>
+      <c r="B87" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>250</v>
+      </c>
+      <c r="B88" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>251</v>
+      </c>
+      <c r="B89" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>252</v>
+      </c>
+      <c r="B90" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>253</v>
+      </c>
+      <c r="B91" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>254</v>
+      </c>
+      <c r="B92" t="s">
+        <v>364</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst1"/>
+    <hyperlink ref="A3" r:id="rId2" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst75"/>
+    <hyperlink ref="A4" r:id="rId3" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst76"/>
+    <hyperlink ref="A5" r:id="rId4" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst77"/>
+    <hyperlink ref="A6" r:id="rId5" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst78"/>
+    <hyperlink ref="A7" r:id="rId6" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst79"/>
+    <hyperlink ref="A8" r:id="rId7" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst80"/>
+    <hyperlink ref="A9" r:id="rId8" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst81"/>
+    <hyperlink ref="A10" r:id="rId9" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst82"/>
+    <hyperlink ref="A11" r:id="rId10" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst83"/>
+    <hyperlink ref="A12" r:id="rId11" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst84"/>
+    <hyperlink ref="A13" r:id="rId12" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst2"/>
+    <hyperlink ref="A14" r:id="rId13" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst3"/>
+    <hyperlink ref="A15" r:id="rId14" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst4"/>
+    <hyperlink ref="A16" r:id="rId15" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst5"/>
+    <hyperlink ref="A17" r:id="rId16" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst85"/>
+    <hyperlink ref="A18" r:id="rId17" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst86"/>
+    <hyperlink ref="A19" r:id="rId18" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst87"/>
+    <hyperlink ref="A20" r:id="rId19" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst88"/>
+    <hyperlink ref="A21" r:id="rId20" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst89"/>
+    <hyperlink ref="A22" r:id="rId21" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst6"/>
+    <hyperlink ref="A23" r:id="rId22" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst7"/>
+    <hyperlink ref="A24" r:id="rId23" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst8"/>
+    <hyperlink ref="A25" r:id="rId24" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst9"/>
+    <hyperlink ref="A26" r:id="rId25" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst10"/>
+    <hyperlink ref="A28" r:id="rId26" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst11"/>
+    <hyperlink ref="A29" r:id="rId27" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst12"/>
+    <hyperlink ref="A30" r:id="rId28" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst13"/>
+    <hyperlink ref="A31" r:id="rId29" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst66"/>
+    <hyperlink ref="A32" r:id="rId30" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst14"/>
+    <hyperlink ref="A33" r:id="rId31" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst96"/>
+    <hyperlink ref="A34" r:id="rId32" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst15"/>
+    <hyperlink ref="A35" r:id="rId33" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst16"/>
+    <hyperlink ref="A36" r:id="rId34" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst17"/>
+    <hyperlink ref="A37" r:id="rId35" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst90"/>
+    <hyperlink ref="A38" r:id="rId36" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst67"/>
+    <hyperlink ref="A39" r:id="rId37" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst18"/>
+    <hyperlink ref="A40" r:id="rId38" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst97"/>
+    <hyperlink ref="A41" r:id="rId39" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst19"/>
+    <hyperlink ref="A42" r:id="rId40" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst20"/>
+    <hyperlink ref="A44" r:id="rId41" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst21"/>
+    <hyperlink ref="A45" r:id="rId42" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst68"/>
+    <hyperlink ref="A46" r:id="rId43" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst22"/>
+    <hyperlink ref="A47" r:id="rId44" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst91"/>
+    <hyperlink ref="A48" r:id="rId45" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst23"/>
+    <hyperlink ref="A49" r:id="rId46" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst24"/>
+    <hyperlink ref="A50" r:id="rId47" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst25"/>
+    <hyperlink ref="A51" r:id="rId48" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst26"/>
+    <hyperlink ref="A52" r:id="rId49" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst28"/>
+    <hyperlink ref="A53" r:id="rId50" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst29"/>
+    <hyperlink ref="A54" r:id="rId51" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst30"/>
+    <hyperlink ref="A56" r:id="rId52" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst31"/>
+    <hyperlink ref="A57" r:id="rId53" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst32"/>
+    <hyperlink ref="A58" r:id="rId54" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst70"/>
+    <hyperlink ref="A59" r:id="rId55" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst71"/>
+    <hyperlink ref="A60" r:id="rId56" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst33"/>
+    <hyperlink ref="A61" r:id="rId57" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst35"/>
+    <hyperlink ref="A62" r:id="rId58" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst34"/>
+    <hyperlink ref="A63" r:id="rId59" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst36"/>
+    <hyperlink ref="A64" r:id="rId60" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst37"/>
+    <hyperlink ref="A65" r:id="rId61" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst38"/>
+    <hyperlink ref="A66" r:id="rId62" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst39"/>
+    <hyperlink ref="A67" r:id="rId63" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst40"/>
+    <hyperlink ref="A68" r:id="rId64" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst41"/>
+    <hyperlink ref="A69" r:id="rId65" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst42"/>
+    <hyperlink ref="A70" r:id="rId66" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst43"/>
+    <hyperlink ref="A71" r:id="rId67" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst72"/>
+    <hyperlink ref="A72" r:id="rId68" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst92"/>
+    <hyperlink ref="A73" r:id="rId69" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst93"/>
+    <hyperlink ref="A74" r:id="rId70" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst44"/>
+    <hyperlink ref="A75" r:id="rId71" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst45"/>
+    <hyperlink ref="A76" r:id="rId72" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst73"/>
+    <hyperlink ref="A77" r:id="rId73" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst74"/>
+    <hyperlink ref="A78" r:id="rId74" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst48"/>
+    <hyperlink ref="A79" r:id="rId75" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst49"/>
+    <hyperlink ref="A80" r:id="rId76" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst50"/>
+    <hyperlink ref="A81" r:id="rId77" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst94"/>
+    <hyperlink ref="A82" r:id="rId78" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst95"/>
+    <hyperlink ref="A83" r:id="rId79" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst52"/>
+    <hyperlink ref="A84" r:id="rId80" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst53"/>
+    <hyperlink ref="A85" r:id="rId81" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst54"/>
+    <hyperlink ref="A86" r:id="rId82" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst55"/>
+    <hyperlink ref="A87" r:id="rId83" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst56"/>
+    <hyperlink ref="A88" r:id="rId84" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst57"/>
+    <hyperlink ref="A89" r:id="rId85" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst58"/>
+    <hyperlink ref="A90" r:id="rId86" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst59"/>
+    <hyperlink ref="A91" r:id="rId87" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst60"/>
+    <hyperlink ref="A92" r:id="rId88" display="http://money.finance.sina.com.cn/corp/view/vFD_FinanceSummaryHistory.php?stockid=300028&amp;typecode=cfst61"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add the title of financial summary
</commit_message>
<xml_diff>
--- a/src/resource/balancesheet-sample.xlsx
+++ b/src/resource/balancesheet-sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="791">
   <si>
     <t>流动资产</t>
   </si>
@@ -2596,6 +2596,18 @@
   </si>
   <si>
     <t>cashequivalentnetincome</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>overallsales</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>notes</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -2783,6 +2795,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2795,7 +2808,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3156,18 +3168,18 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>257</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="26" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="20.25" customHeight="1">
@@ -3896,18 +3908,18 @@
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="26" t="s">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9">
@@ -4694,18 +4706,18 @@
       </c>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="26" t="s">
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9">
@@ -5637,18 +5649,18 @@
       </c>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="24" t="s">
+      <c r="A90" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="24" t="s">
+      <c r="B90" s="26"/>
+      <c r="C90" s="26"/>
+      <c r="D90" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="25"/>
-      <c r="H90" s="25"/>
+      <c r="E90" s="26"/>
+      <c r="F90" s="26"/>
+      <c r="G90" s="26"/>
+      <c r="H90" s="26"/>
       <c r="I90" s="1"/>
     </row>
     <row r="91" spans="1:9">
@@ -5913,18 +5925,18 @@
       </c>
     </row>
     <row r="100" spans="1:9">
-      <c r="A100" s="24" t="s">
+      <c r="A100" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="B100" s="25"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="24" t="s">
+      <c r="B100" s="26"/>
+      <c r="C100" s="26"/>
+      <c r="D100" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25"/>
-      <c r="H100" s="25"/>
+      <c r="E100" s="26"/>
+      <c r="F100" s="26"/>
+      <c r="G100" s="26"/>
+      <c r="H100" s="26"/>
       <c r="I100" s="1"/>
     </row>
     <row r="101" spans="1:9">
@@ -9441,8 +9453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -10236,10 +10248,10 @@
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="28" t="s">
+      <c r="A72" s="24" t="s">
         <v>603</v>
       </c>
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="24" t="s">
         <v>604</v>
       </c>
       <c r="C72" t="s">
@@ -10269,10 +10281,10 @@
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="28" t="s">
+      <c r="A75" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="28" t="s">
+      <c r="B75" s="24" t="s">
         <v>306</v>
       </c>
       <c r="C75" t="s">
@@ -10818,7 +10830,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -10848,6 +10860,9 @@
       <c r="B2" s="23" t="s">
         <v>407</v>
       </c>
+      <c r="C2" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
@@ -11387,8 +11402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -12008,6 +12023,12 @@
     <row r="56" spans="1:3">
       <c r="A56" s="17" t="s">
         <v>219</v>
+      </c>
+      <c r="B56" t="s">
+        <v>789</v>
+      </c>
+      <c r="C56" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="57" spans="1:3">

</xml_diff>